<commit_message>
Qr item approvement added
</commit_message>
<xml_diff>
--- a/reports/items_report.xlsx
+++ b/reports/items_report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Отчет по инвентарю" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,67 +429,32 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Наименование объекта</t>
+          <t>Наименование объекта нефинансового учета</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Номер объекта учета</t>
+          <t>Номер(код) объекта учета</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Оценочная стоимость</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Количество</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Сумма</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Статус объекта учета</t>
+          <t>Фактическое наличие</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Оценочное количество</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Балансовая стоимость</t>
+          <t>По данным бухгалтерского учета</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Количество недостача</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Сумма недосдачи</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Количество излишков</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Сумма излишков</t>
+          <t>Результаты инвентаризации</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Финансово ответственное лицо</t>
+          <t>Материально ответственное лицо</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
@@ -499,63 +464,206 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Отклонение</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Цена(оценочная стоимость), руб</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Количество</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Сумма, руб</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Статус объекта учета</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Количество</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Балансовая стоимость, руб</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Недосдача</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Излишки</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Количество</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Сумма, руб</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Количество</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Сумма, руб</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>chair</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>inventarid</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>статус</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>20</v>
-      </c>
-      <c r="I2" t="n">
-        <v>200</v>
-      </c>
-      <c r="J2" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-10</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-2000</v>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>В работе</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>prop</t>
-        </is>
-      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>sgdfgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>В работе</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="N1:N4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="J1:M1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QR path fix and quality of life features
</commit_message>
<xml_diff>
--- a/reports/items_report.xlsx
+++ b/reports/items_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,116 +533,6 @@
           <t>Сумма, руб</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Placeholder</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>В работе</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>sgdfgd</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Placeholder</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>В работе</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>

<commit_message>
Reports view sorts initialized
</commit_message>
<xml_diff>
--- a/reports/items_report.xlsx
+++ b/reports/items_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,120 @@
       <c r="M4" t="inlineStr">
         <is>
           <t>Сумма, руб</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>В работе</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>На месте</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>В работе</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Все просрано</t>
         </is>
       </c>
     </row>

</xml_diff>